<commit_message>
Fixed ALLOWED_HOSTS and Static files
</commit_message>
<xml_diff>
--- a/travel_agency/travel_app/storage/bookings.xlsx
+++ b/travel_agency/travel_app/storage/bookings.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1600,6 +1600,80 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Anil Prasad</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>kumarr47872@gmail.com</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-02-18</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-02-17 23:05:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>RAHUL KUMAR</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>231fa04862@gmail.com</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-02-19</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing </t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-02-17 23:12:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>